<commit_message>
Subo pila semanal corregida, riesgos y seguimiento
</commit_message>
<xml_diff>
--- a/1-Planificacion/Pilas del Sprint 1/Plantilla Pila de Sprint semana2.xlsx
+++ b/1-Planificacion/Pilas del Sprint 1/Plantilla Pila de Sprint semana2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="75">
   <si>
     <t>CATEGORÍA</t>
   </si>
@@ -128,73 +128,139 @@
     <t>EspecificaciÓn de Casos de Uso</t>
   </si>
   <si>
-    <t>Gestion</t>
-  </si>
-  <si>
-    <t>Instalacion de herramientas de desarrollo</t>
-  </si>
-  <si>
-    <t>Alejandro Betancourth</t>
-  </si>
-  <si>
-    <t>Equipos de computo</t>
-  </si>
-  <si>
-    <t>Equipo computo fucionando como servidor local</t>
-  </si>
-  <si>
-    <t>Lecturas de dcumentos(herramientas de desarrollo)</t>
-  </si>
-  <si>
-    <t>Meida</t>
-  </si>
-  <si>
-    <t>Ruben Acuña</t>
-  </si>
-  <si>
-    <t>Libros, WEB</t>
-  </si>
-  <si>
-    <t>Informe de lectura e investigacion</t>
-  </si>
-  <si>
-    <t>Semanal</t>
-  </si>
-  <si>
     <t>En ejecucion</t>
   </si>
   <si>
-    <t>Elaboracion de documentos</t>
-  </si>
-  <si>
-    <t>Media</t>
-  </si>
-  <si>
-    <t>Plantilla</t>
-  </si>
-  <si>
-    <t>Documento de texto</t>
-  </si>
-  <si>
-    <t>Actas de reuniones</t>
-  </si>
-  <si>
-    <t>Baja</t>
-  </si>
-  <si>
-    <t>Implementacion</t>
-  </si>
-  <si>
-    <t>Instalacion de manejador de base de datos</t>
-  </si>
-  <si>
-    <t>WAMP server</t>
-  </si>
-  <si>
-    <t>Equipo computo fucionando como servidor local e ingreso al motor de base de datos</t>
-  </si>
-  <si>
     <t>Atrasado</t>
+  </si>
+  <si>
+    <t>ANALISIS</t>
+  </si>
+  <si>
+    <t>ESPECIFICACION CASOS DE USO</t>
+  </si>
+  <si>
+    <t>DIAGRAMAS CASOS DE USO</t>
+  </si>
+  <si>
+    <t>MOCKUPS</t>
+  </si>
+  <si>
+    <t>SEGUIMIENTO</t>
+  </si>
+  <si>
+    <t>DOCUMENTO ACTA DE REUNIONES</t>
+  </si>
+  <si>
+    <t>DISEÑO</t>
+  </si>
+  <si>
+    <t>DIAGRAMA DE CLASES</t>
+  </si>
+  <si>
+    <t>ALTA</t>
+  </si>
+  <si>
+    <t>DIAGRAMA ENTIDAD RELACION</t>
+  </si>
+  <si>
+    <t>MODELO ARQUITECTONICO (MVC - WEB)</t>
+  </si>
+  <si>
+    <t>DESCRIPCION DE LA BASE DE DATOS</t>
+  </si>
+  <si>
+    <t>MEDIO</t>
+  </si>
+  <si>
+    <t>MODELO DE BASE DE DATOS</t>
+  </si>
+  <si>
+    <t>IMPLEMENTACION</t>
+  </si>
+  <si>
+    <t>CREACION DE LAYOUT Y ESTILO DE SITIO WEB</t>
+  </si>
+  <si>
+    <t>CREAR PAGINA PRINCIPAL</t>
+  </si>
+  <si>
+    <t>CREAR VALIDADOR DE USUARIOS</t>
+  </si>
+  <si>
+    <t>CREAR CATEGORIA</t>
+  </si>
+  <si>
+    <t>GUARDAR ARTICULO/PRODUCTO</t>
+  </si>
+  <si>
+    <t>PRUEBAS</t>
+  </si>
+  <si>
+    <t>DOCUMENTO ESPECIFICACION DE PRUEBAS VALIDACION DE USUARIO</t>
+  </si>
+  <si>
+    <t>MODO DE EJECUCION DE PRUEBAS VALIDACION DE USUARIO</t>
+  </si>
+  <si>
+    <t>DOCUMENTO DE RESULTADO DE PRUEBAS VALIDACION DE USUARIO</t>
+  </si>
+  <si>
+    <t>DOCUMENTO ESPECIFICACION DE PRUEBAS CREACION DEL PRODUCTO</t>
+  </si>
+  <si>
+    <t>IMPLANTACION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MANUAL DE USUARIO </t>
+  </si>
+  <si>
+    <t>GESTION</t>
+  </si>
+  <si>
+    <t>SEGUNDA REVISION DE CALIDAD</t>
+  </si>
+  <si>
+    <t>BAJA</t>
+  </si>
+  <si>
+    <t>JUAN P. CAMPOS</t>
+  </si>
+  <si>
+    <t>CAMILO AGUDELO</t>
+  </si>
+  <si>
+    <t>ALEJANDRO BETANCOURTH</t>
+  </si>
+  <si>
+    <t>JOSE TANGARIFE</t>
+  </si>
+  <si>
+    <t>RUBEN ACUÑA</t>
+  </si>
+  <si>
+    <t>PLANTILLA</t>
+  </si>
+  <si>
+    <t>Equipo de computo</t>
+  </si>
+  <si>
+    <t>WORD</t>
+  </si>
+  <si>
+    <t>DOCUMENTO</t>
+  </si>
+  <si>
+    <t>Aplicativo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Documento </t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>semanal</t>
   </si>
 </sst>
 </file>
@@ -249,7 +315,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -598,11 +664,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -691,10 +781,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -703,6 +805,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -712,32 +817,23 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1019,24 +1115,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:P47"/>
+  <dimension ref="B1:P58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="5.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.28515625" style="1" customWidth="1"/>
     <col min="12" max="12" width="12.85546875" style="1" customWidth="1"/>
     <col min="13" max="16" width="7.85546875" style="1" customWidth="1"/>
@@ -1045,58 +1141,58 @@
   <sheetData>
     <row r="1" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="40" t="s">
+      <c r="E2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="35" t="s">
+      <c r="F2" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="40" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="32" t="s">
+      <c r="G2" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="32" t="s">
+      <c r="I2" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="34" t="s">
+      <c r="J2" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="35" t="s">
+      <c r="K2" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="37" t="s">
+      <c r="L2" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="39" t="s">
+      <c r="M2" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="41"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="34"/>
     </row>
     <row r="3" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="45"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="38"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="31"/>
       <c r="M3" s="2" t="s">
         <v>10</v>
       </c>
@@ -1304,7 +1400,7 @@
         <v>42821</v>
       </c>
       <c r="J8" s="22" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="K8" s="20">
         <v>4</v>
@@ -1338,58 +1434,58 @@
       <c r="P9" s="15"/>
     </row>
     <row r="10" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="44" t="s">
+      <c r="B10" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="35" t="s">
+      <c r="C10" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="40" t="s">
+      <c r="D10" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="E10" s="40" t="s">
+      <c r="E10" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="F10" s="35" t="s">
+      <c r="F10" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="G10" s="40" t="s">
-        <v>4</v>
-      </c>
-      <c r="H10" s="32" t="s">
+      <c r="G10" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="I10" s="32" t="s">
+      <c r="I10" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="J10" s="34" t="s">
+      <c r="J10" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="K10" s="35" t="s">
+      <c r="K10" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="L10" s="37" t="s">
+      <c r="L10" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="M10" s="39" t="s">
+      <c r="M10" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="N10" s="40"/>
-      <c r="O10" s="40"/>
-      <c r="P10" s="41"/>
+      <c r="N10" s="33"/>
+      <c r="O10" s="33"/>
+      <c r="P10" s="34"/>
     </row>
     <row r="11" spans="2:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="45"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="42"/>
-      <c r="J11" s="33"/>
-      <c r="K11" s="36"/>
-      <c r="L11" s="38"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="37"/>
+      <c r="K11" s="41"/>
+      <c r="L11" s="31"/>
       <c r="M11" s="2" t="s">
         <v>10</v>
       </c>
@@ -1403,19 +1499,19 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="2:16" ht="26.25" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="31"/>
+    <row r="12" spans="2:16" ht="13.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="45"/>
       <c r="C12" s="7" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>26</v>
@@ -1423,39 +1519,39 @@
       <c r="H12" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="I12" s="13">
-        <v>42821</v>
+      <c r="I12" s="13" t="s">
+        <v>74</v>
       </c>
       <c r="J12" s="27" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="K12" s="7">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="L12" s="10">
-        <f t="shared" ref="L12:L15" si="1">K12-(SUM(M12:P12))</f>
-        <v>3</v>
+        <f t="shared" ref="L12:L31" si="1">K12-(SUM(M12:P12))</f>
+        <v>12</v>
       </c>
       <c r="M12" s="11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="N12" s="7"/>
       <c r="O12" s="7"/>
       <c r="P12" s="12"/>
     </row>
-    <row r="13" spans="2:16" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B13" s="31"/>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B13" s="46"/>
       <c r="C13" s="7" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>26</v>
@@ -1463,500 +1559,735 @@
       <c r="H13" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="I13" s="13">
-        <v>42821</v>
+      <c r="I13" s="13" t="s">
+        <v>74</v>
       </c>
       <c r="J13" s="27" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="K13" s="7">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="L13" s="10">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="M13" s="11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="N13" s="7"/>
       <c r="O13" s="7"/>
       <c r="P13" s="12"/>
     </row>
-    <row r="14" spans="2:16" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B14" s="31"/>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B14" s="46"/>
       <c r="C14" s="7" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="I14" s="13">
-        <v>42821</v>
+        <v>35</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>74</v>
       </c>
       <c r="J14" s="27" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="K14" s="7">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="L14" s="10">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="M14" s="11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="N14" s="7"/>
       <c r="O14" s="7"/>
       <c r="P14" s="12"/>
     </row>
-    <row r="15" spans="2:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="31"/>
+    <row r="15" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="46"/>
       <c r="C15" s="20" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="F15" s="20" t="s">
-        <v>19</v>
+        <v>40</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>66</v>
       </c>
       <c r="G15" s="20" t="s">
-        <v>26</v>
+        <v>67</v>
       </c>
       <c r="H15" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="I15" s="21">
-        <v>42821</v>
+        <v>70</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>74</v>
       </c>
       <c r="J15" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="K15" s="20">
-        <v>4</v>
-      </c>
-      <c r="L15" s="23">
+        <v>30</v>
+      </c>
+      <c r="K15" s="7">
+        <v>16</v>
+      </c>
+      <c r="L15" s="10">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="M15" s="24">
-        <v>1</v>
+        <v>12</v>
+      </c>
+      <c r="M15" s="11">
+        <v>4</v>
       </c>
       <c r="N15" s="20"/>
       <c r="O15" s="20"/>
       <c r="P15" s="25"/>
     </row>
-    <row r="16" spans="2:16" ht="51" x14ac:dyDescent="0.25">
-      <c r="B16" s="8">
-        <v>1</v>
-      </c>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B16" s="47"/>
       <c r="C16" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="J16" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="E16" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="F16" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="G16" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="H16" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="I16" s="13">
-        <v>42824</v>
-      </c>
-      <c r="J16" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="K16" s="26">
-        <v>2</v>
+      <c r="K16" s="7">
+        <v>16</v>
       </c>
       <c r="L16" s="10">
-        <f t="shared" ref="L16:L20" si="2">K16-(SUM(M16:P16))</f>
-        <v>2</v>
-      </c>
-      <c r="M16" s="28"/>
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="M16" s="11">
+        <v>4</v>
+      </c>
       <c r="N16" s="26"/>
       <c r="O16" s="26"/>
       <c r="P16" s="29"/>
     </row>
-    <row r="17" spans="2:16" ht="51" x14ac:dyDescent="0.25">
-      <c r="B17" s="8">
-        <v>2</v>
-      </c>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B17" s="8"/>
       <c r="C17" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="G17" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="J17" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="F17" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="G17" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="H17" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="I17" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="J17" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="K17" s="26">
-        <v>6</v>
+      <c r="K17" s="7">
+        <v>16</v>
       </c>
       <c r="L17" s="10">
-        <f t="shared" si="2"/>
-        <v>4.5</v>
-      </c>
-      <c r="M17" s="28">
-        <v>1.5</v>
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="M17" s="11">
+        <v>4</v>
       </c>
       <c r="N17" s="26"/>
       <c r="O17" s="26"/>
       <c r="P17" s="29"/>
     </row>
-    <row r="18" spans="2:16" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="8">
-        <v>3</v>
-      </c>
+    <row r="18" spans="2:16" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B18" s="8"/>
       <c r="C18" s="26" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D18" s="26" t="s">
         <v>42</v>
       </c>
       <c r="E18" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>23</v>
+        <v>40</v>
+      </c>
+      <c r="F18" s="26" t="s">
+        <v>63</v>
       </c>
       <c r="G18" s="26" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="H18" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="I18" s="27" t="s">
-        <v>40</v>
+        <v>27</v>
+      </c>
+      <c r="I18" s="13" t="s">
+        <v>74</v>
       </c>
       <c r="J18" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="K18" s="26">
-        <v>4</v>
+        <v>30</v>
+      </c>
+      <c r="K18" s="7">
+        <v>16</v>
       </c>
       <c r="L18" s="10">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="M18" s="28">
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="M18" s="11">
+        <v>4</v>
       </c>
       <c r="N18" s="26"/>
       <c r="O18" s="26"/>
       <c r="P18" s="29"/>
     </row>
     <row r="19" spans="2:16" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B19" s="8">
-        <v>4</v>
-      </c>
+      <c r="B19" s="8"/>
       <c r="C19" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="G19" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="H19" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="J19" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="E19" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="F19" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="G19" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="H19" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="I19" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="J19" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="K19" s="26">
-        <v>2</v>
+      <c r="K19" s="7">
+        <v>16</v>
       </c>
       <c r="L19" s="10">
-        <f t="shared" si="2"/>
-        <v>1.5</v>
-      </c>
-      <c r="M19" s="28">
-        <v>0.5</v>
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="M19" s="11">
+        <v>4</v>
       </c>
       <c r="N19" s="26"/>
       <c r="O19" s="26"/>
       <c r="P19" s="29"/>
     </row>
-    <row r="20" spans="2:16" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="19">
-        <v>5</v>
-      </c>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B20" s="8"/>
       <c r="C20" s="26" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D20" s="26" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E20" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>24</v>
+        <v>40</v>
+      </c>
+      <c r="F20" s="26" t="s">
+        <v>63</v>
       </c>
       <c r="G20" s="26" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="H20" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="I20" s="30">
-        <v>42828</v>
+        <v>27</v>
+      </c>
+      <c r="I20" s="13" t="s">
+        <v>74</v>
       </c>
       <c r="J20" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="K20" s="26">
-        <v>0.5</v>
+        <v>30</v>
+      </c>
+      <c r="K20" s="7">
+        <v>16</v>
       </c>
       <c r="L20" s="10">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="M20" s="28"/>
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="M20" s="11">
+        <v>4</v>
+      </c>
       <c r="N20" s="26"/>
       <c r="O20" s="26"/>
       <c r="P20" s="29"/>
     </row>
-    <row r="21" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="16"/>
-      <c r="M21" s="15"/>
-      <c r="N21" s="15"/>
-      <c r="O21" s="15"/>
-      <c r="P21" s="15"/>
-    </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="16"/>
-      <c r="M22" s="15"/>
-      <c r="N22" s="15"/>
-      <c r="O22" s="15"/>
-      <c r="P22" s="15"/>
-    </row>
-    <row r="23" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="15"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="16"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="15"/>
-      <c r="P23" s="15"/>
-    </row>
-    <row r="24" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="16"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
-      <c r="O24" s="15"/>
-      <c r="P24" s="15"/>
-    </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="17"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="15"/>
-      <c r="L25" s="16"/>
-      <c r="M25" s="15"/>
-      <c r="N25" s="15"/>
-      <c r="O25" s="15"/>
-      <c r="P25" s="15"/>
-    </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="17"/>
-      <c r="J26" s="15"/>
-      <c r="K26" s="15"/>
-      <c r="L26" s="16"/>
-      <c r="M26" s="15"/>
-      <c r="N26" s="15"/>
-      <c r="O26" s="15"/>
-      <c r="P26" s="15"/>
-    </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
-      <c r="I27" s="17"/>
-      <c r="J27" s="15"/>
-      <c r="K27" s="15"/>
-      <c r="L27" s="16"/>
-      <c r="M27" s="15"/>
-      <c r="N27" s="15"/>
-      <c r="O27" s="15"/>
-      <c r="P27" s="15"/>
-    </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="15"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="16"/>
-      <c r="M28" s="15"/>
-      <c r="N28" s="15"/>
-      <c r="O28" s="15"/>
-      <c r="P28" s="15"/>
-    </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="17"/>
-      <c r="J29" s="15"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="16"/>
-      <c r="M29" s="15"/>
-      <c r="N29" s="15"/>
-      <c r="O29" s="15"/>
-      <c r="P29" s="15"/>
+    <row r="21" spans="2:16" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B21" s="8"/>
+      <c r="C21" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="G21" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="H21" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="I21" s="13">
+        <v>42828</v>
+      </c>
+      <c r="J21" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="K21" s="26">
+        <v>4</v>
+      </c>
+      <c r="L21" s="10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="M21" s="28"/>
+      <c r="N21" s="26"/>
+      <c r="O21" s="26"/>
+      <c r="P21" s="29"/>
+    </row>
+    <row r="22" spans="2:16" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B22" s="8"/>
+      <c r="C22" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="G22" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="H22" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="I22" s="13">
+        <v>42828</v>
+      </c>
+      <c r="J22" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="K22" s="26">
+        <v>4</v>
+      </c>
+      <c r="L22" s="10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="M22" s="28"/>
+      <c r="N22" s="26"/>
+      <c r="O22" s="26"/>
+      <c r="P22" s="29"/>
+    </row>
+    <row r="23" spans="2:16" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B23" s="8"/>
+      <c r="C23" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="F23" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="G23" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="H23" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="I23" s="13">
+        <v>42828</v>
+      </c>
+      <c r="J23" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="K23" s="26">
+        <v>4</v>
+      </c>
+      <c r="L23" s="10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="M23" s="28"/>
+      <c r="N23" s="26"/>
+      <c r="O23" s="26"/>
+      <c r="P23" s="29"/>
+    </row>
+    <row r="24" spans="2:16" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B24" s="8"/>
+      <c r="C24" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="F24" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="G24" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="H24" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="I24" s="13">
+        <v>42828</v>
+      </c>
+      <c r="J24" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="K24" s="26">
+        <v>4</v>
+      </c>
+      <c r="L24" s="10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="M24" s="28"/>
+      <c r="N24" s="26"/>
+      <c r="O24" s="26"/>
+      <c r="P24" s="29"/>
+    </row>
+    <row r="25" spans="2:16" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B25" s="8"/>
+      <c r="C25" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="E25" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="F25" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="G25" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="H25" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="I25" s="13">
+        <v>42828</v>
+      </c>
+      <c r="J25" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="K25" s="26">
+        <v>4</v>
+      </c>
+      <c r="L25" s="10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="M25" s="28"/>
+      <c r="N25" s="26"/>
+      <c r="O25" s="26"/>
+      <c r="P25" s="29"/>
+    </row>
+    <row r="26" spans="2:16" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B26" s="8"/>
+      <c r="C26" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="E26" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="F26" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="G26" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="H26" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="I26" s="13">
+        <v>42828</v>
+      </c>
+      <c r="J26" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="K26" s="26">
+        <v>2</v>
+      </c>
+      <c r="L26" s="10">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="M26" s="28"/>
+      <c r="N26" s="26"/>
+      <c r="O26" s="26"/>
+      <c r="P26" s="29"/>
+    </row>
+    <row r="27" spans="2:16" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B27" s="8">
+        <v>2</v>
+      </c>
+      <c r="C27" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="E27" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="F27" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="G27" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="H27" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="I27" s="13">
+        <v>42828</v>
+      </c>
+      <c r="J27" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="K27" s="26">
+        <v>2</v>
+      </c>
+      <c r="L27" s="10">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="M27" s="28"/>
+      <c r="N27" s="26"/>
+      <c r="O27" s="26"/>
+      <c r="P27" s="29"/>
+    </row>
+    <row r="28" spans="2:16" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B28" s="8">
+        <v>3</v>
+      </c>
+      <c r="C28" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="E28" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="F28" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="G28" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="H28" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="I28" s="13">
+        <v>42828</v>
+      </c>
+      <c r="J28" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="K28" s="26">
+        <v>2</v>
+      </c>
+      <c r="L28" s="10">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="M28" s="28"/>
+      <c r="N28" s="26"/>
+      <c r="O28" s="26"/>
+      <c r="P28" s="29"/>
+    </row>
+    <row r="29" spans="2:16" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B29" s="8">
+        <v>4</v>
+      </c>
+      <c r="C29" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="E29" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="F29" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="G29" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="H29" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="I29" s="13">
+        <v>42828</v>
+      </c>
+      <c r="J29" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="K29" s="26">
+        <v>2</v>
+      </c>
+      <c r="L29" s="10">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="M29" s="28"/>
+      <c r="N29" s="26"/>
+      <c r="O29" s="26"/>
+      <c r="P29" s="29"/>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B30" s="15"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="15"/>
-      <c r="I30" s="17"/>
-      <c r="J30" s="15"/>
-      <c r="K30" s="15"/>
-      <c r="L30" s="16"/>
-      <c r="M30" s="15"/>
-      <c r="N30" s="15"/>
-      <c r="O30" s="15"/>
-      <c r="P30" s="15"/>
-    </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B31" s="15"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="15"/>
-      <c r="I31" s="17"/>
-      <c r="J31" s="15"/>
-      <c r="K31" s="15"/>
-      <c r="L31" s="16"/>
-      <c r="M31" s="15"/>
-      <c r="N31" s="15"/>
-      <c r="O31" s="15"/>
-      <c r="P31" s="15"/>
-    </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B30" s="44"/>
+      <c r="C30" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="D30" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="E30" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="G30" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="H30" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="I30" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="J30" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="K30" s="26">
+        <v>16</v>
+      </c>
+      <c r="L30" s="10">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="M30" s="28">
+        <v>4</v>
+      </c>
+      <c r="N30" s="26"/>
+      <c r="O30" s="26"/>
+      <c r="P30" s="29"/>
+    </row>
+    <row r="31" spans="2:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="19">
+        <v>5</v>
+      </c>
+      <c r="C31" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D31" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="E31" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="G31" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="H31" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="I31" s="13">
+        <v>42828</v>
+      </c>
+      <c r="J31" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="K31" s="26">
+        <v>4</v>
+      </c>
+      <c r="L31" s="10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="M31" s="28"/>
+      <c r="N31" s="26"/>
+      <c r="O31" s="26"/>
+      <c r="P31" s="29"/>
+    </row>
+    <row r="32" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="15"/>
       <c r="C32" s="15"/>
       <c r="D32" s="15"/>
@@ -1981,7 +2312,7 @@
       <c r="F33" s="15"/>
       <c r="G33" s="15"/>
       <c r="H33" s="15"/>
-      <c r="I33" s="17"/>
+      <c r="I33" s="15"/>
       <c r="J33" s="15"/>
       <c r="K33" s="15"/>
       <c r="L33" s="16"/>
@@ -1990,7 +2321,7 @@
       <c r="O33" s="15"/>
       <c r="P33" s="15"/>
     </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
       <c r="D34" s="15"/>
@@ -1998,7 +2329,7 @@
       <c r="F34" s="15"/>
       <c r="G34" s="15"/>
       <c r="H34" s="15"/>
-      <c r="I34" s="17"/>
+      <c r="I34" s="15"/>
       <c r="J34" s="15"/>
       <c r="K34" s="15"/>
       <c r="L34" s="16"/>
@@ -2007,7 +2338,7 @@
       <c r="O34" s="15"/>
       <c r="P34" s="15"/>
     </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
       <c r="D35" s="15"/>
@@ -2059,68 +2390,272 @@
       <c r="P37" s="15"/>
     </row>
     <row r="38" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="18"/>
-      <c r="H38" s="18"/>
-      <c r="I38" s="18"/>
-      <c r="J38" s="18"/>
-      <c r="K38" s="18"/>
-      <c r="L38" s="18"/>
-      <c r="M38" s="18"/>
-      <c r="N38" s="18"/>
-      <c r="O38" s="18"/>
-      <c r="P38" s="18"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="17"/>
+      <c r="J38" s="15"/>
+      <c r="K38" s="15"/>
+      <c r="L38" s="16"/>
+      <c r="M38" s="15"/>
+      <c r="N38" s="15"/>
+      <c r="O38" s="15"/>
+      <c r="P38" s="15"/>
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B39" s="18"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="18"/>
-      <c r="H39" s="18"/>
-      <c r="I39" s="18"/>
-      <c r="J39" s="18"/>
-      <c r="K39" s="18"/>
-      <c r="L39" s="18"/>
-      <c r="M39" s="18"/>
-      <c r="N39" s="18"/>
-      <c r="O39" s="18"/>
-      <c r="P39" s="18"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="15"/>
+      <c r="I39" s="15"/>
+      <c r="J39" s="15"/>
+      <c r="K39" s="15"/>
+      <c r="L39" s="16"/>
+      <c r="M39" s="15"/>
+      <c r="N39" s="15"/>
+      <c r="O39" s="15"/>
+      <c r="P39" s="15"/>
     </row>
     <row r="40" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C40" s="6"/>
-      <c r="D40" s="5"/>
-      <c r="J40" s="6"/>
-      <c r="L40" s="6"/>
+      <c r="B40" s="15"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="15"/>
+      <c r="I40" s="17"/>
+      <c r="J40" s="15"/>
+      <c r="K40" s="15"/>
+      <c r="L40" s="16"/>
+      <c r="M40" s="15"/>
+      <c r="N40" s="15"/>
+      <c r="O40" s="15"/>
+      <c r="P40" s="15"/>
     </row>
     <row r="41" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D41" s="5"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="15"/>
+      <c r="I41" s="17"/>
+      <c r="J41" s="15"/>
+      <c r="K41" s="15"/>
+      <c r="L41" s="16"/>
+      <c r="M41" s="15"/>
+      <c r="N41" s="15"/>
+      <c r="O41" s="15"/>
+      <c r="P41" s="15"/>
     </row>
     <row r="42" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D42" s="5"/>
+      <c r="B42" s="15"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="15"/>
+      <c r="I42" s="17"/>
+      <c r="J42" s="15"/>
+      <c r="K42" s="15"/>
+      <c r="L42" s="16"/>
+      <c r="M42" s="15"/>
+      <c r="N42" s="15"/>
+      <c r="O42" s="15"/>
+      <c r="P42" s="15"/>
     </row>
     <row r="43" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D43" s="5"/>
+      <c r="B43" s="15"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="15"/>
+      <c r="I43" s="17"/>
+      <c r="J43" s="15"/>
+      <c r="K43" s="15"/>
+      <c r="L43" s="16"/>
+      <c r="M43" s="15"/>
+      <c r="N43" s="15"/>
+      <c r="O43" s="15"/>
+      <c r="P43" s="15"/>
     </row>
     <row r="44" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D44" s="5"/>
+      <c r="B44" s="15"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="15"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="15"/>
+      <c r="H44" s="15"/>
+      <c r="I44" s="17"/>
+      <c r="J44" s="15"/>
+      <c r="K44" s="15"/>
+      <c r="L44" s="16"/>
+      <c r="M44" s="15"/>
+      <c r="N44" s="15"/>
+      <c r="O44" s="15"/>
+      <c r="P44" s="15"/>
     </row>
     <row r="45" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D45" s="5"/>
+      <c r="B45" s="15"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="15"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="15"/>
+      <c r="H45" s="15"/>
+      <c r="I45" s="17"/>
+      <c r="J45" s="15"/>
+      <c r="K45" s="15"/>
+      <c r="L45" s="16"/>
+      <c r="M45" s="15"/>
+      <c r="N45" s="15"/>
+      <c r="O45" s="15"/>
+      <c r="P45" s="15"/>
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D46" s="5"/>
+      <c r="B46" s="15"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="15"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="15"/>
+      <c r="H46" s="15"/>
+      <c r="I46" s="15"/>
+      <c r="J46" s="15"/>
+      <c r="K46" s="15"/>
+      <c r="L46" s="16"/>
+      <c r="M46" s="15"/>
+      <c r="N46" s="15"/>
+      <c r="O46" s="15"/>
+      <c r="P46" s="15"/>
     </row>
     <row r="47" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D47" s="5"/>
+      <c r="B47" s="15"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="15"/>
+      <c r="F47" s="15"/>
+      <c r="G47" s="15"/>
+      <c r="H47" s="15"/>
+      <c r="I47" s="17"/>
+      <c r="J47" s="15"/>
+      <c r="K47" s="15"/>
+      <c r="L47" s="16"/>
+      <c r="M47" s="15"/>
+      <c r="N47" s="15"/>
+      <c r="O47" s="15"/>
+      <c r="P47" s="15"/>
+    </row>
+    <row r="48" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B48" s="15"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="15"/>
+      <c r="E48" s="15"/>
+      <c r="F48" s="15"/>
+      <c r="G48" s="15"/>
+      <c r="H48" s="15"/>
+      <c r="I48" s="17"/>
+      <c r="J48" s="15"/>
+      <c r="K48" s="15"/>
+      <c r="L48" s="16"/>
+      <c r="M48" s="15"/>
+      <c r="N48" s="15"/>
+      <c r="O48" s="15"/>
+      <c r="P48" s="15"/>
+    </row>
+    <row r="49" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B49" s="18"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="18"/>
+      <c r="G49" s="18"/>
+      <c r="H49" s="18"/>
+      <c r="I49" s="18"/>
+      <c r="J49" s="18"/>
+      <c r="K49" s="18"/>
+      <c r="L49" s="18"/>
+      <c r="M49" s="18"/>
+      <c r="N49" s="18"/>
+      <c r="O49" s="18"/>
+      <c r="P49" s="18"/>
+    </row>
+    <row r="50" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B50" s="18"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="18"/>
+      <c r="G50" s="18"/>
+      <c r="H50" s="18"/>
+      <c r="I50" s="18"/>
+      <c r="J50" s="18"/>
+      <c r="K50" s="18"/>
+      <c r="L50" s="18"/>
+      <c r="M50" s="18"/>
+      <c r="N50" s="18"/>
+      <c r="O50" s="18"/>
+      <c r="P50" s="18"/>
+    </row>
+    <row r="51" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C51" s="6"/>
+      <c r="D51" s="5"/>
+      <c r="J51" s="6"/>
+      <c r="L51" s="6"/>
+    </row>
+    <row r="52" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D52" s="5"/>
+    </row>
+    <row r="53" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D53" s="5"/>
+    </row>
+    <row r="54" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D54" s="5"/>
+    </row>
+    <row r="55" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D55" s="5"/>
+    </row>
+    <row r="56" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D56" s="5"/>
+    </row>
+    <row r="57" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D57" s="5"/>
+    </row>
+    <row r="58" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D58" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
     <mergeCell ref="L10:L11"/>
     <mergeCell ref="M10:P10"/>
     <mergeCell ref="G10:G11"/>
@@ -2128,23 +2663,6 @@
     <mergeCell ref="I10:I11"/>
     <mergeCell ref="J10:J11"/>
     <mergeCell ref="K10:K11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="M2:P2"/>
-    <mergeCell ref="I2:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>